<commit_message>
Updated RPA Challenge Code
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
+++ b/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b217b7127be6c014/Documents/RPA30Days_Program/RPA-Developer-in-30-Days/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98571280-E612-4411-88EB-51E45C25DA69}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Robot1</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -598,7 +601,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2782,7 +2787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Project_Updated RPAChallenge Code, Package & Deployment Sheet
Project_Updated RPAChallenge Code, Package & Deployment Sheet
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
+++ b/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b217b7127be6c014/Documents/RPA30Days_Program/RPA-Developer-in-30-Days/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98571280-E612-4411-88EB-51E45C25DA69}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5A5092D-5C29-4E0B-A5A2-153DA11E7CBF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -98,78 +98,92 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Robot1</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Orchestrator_FolderName</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>Robot1</t>
+  </si>
+  <si>
+    <t>RPAChallenge_URL</t>
+  </si>
+  <si>
+    <t>RPAChallenge_Path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +207,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -224,6 +244,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,6 +260,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -588,10 +621,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -599,13 +632,13 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -620,10 +653,38 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1678,18 +1739,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1713,7 +1774,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1735,7 +1796,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1746,7 +1807,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1757,53 +1818,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2787,7 +2848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2805,7 +2868,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Project_Updated Code, Package & Deployment Sheet
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
+++ b/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b217b7127be6c014/Documents/RPA30Days_Program/RPA-Developer-in-30-Days/SourceCode/2023/August2023/Yash/RE_RPAChallenge/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5A5092D-5C29-4E0B-A5A2-153DA11E7CBF}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8D777FB-C583-4694-ABE0-55CC7F109579}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -158,18 +158,12 @@
     <t>ProcessABCQueue</t>
   </si>
   <si>
-    <t>Robot1</t>
-  </si>
-  <si>
     <t>SheetName</t>
   </si>
   <si>
     <t>Sheet1</t>
   </si>
   <si>
-    <t>Orchestrator_FolderName</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -177,6 +171,9 @@
   </si>
   <si>
     <t>RPAChallenge_Path</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
@@ -271,6 +268,14 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -574,7 +579,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -621,7 +626,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>43</v>
@@ -635,7 +640,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -655,34 +660,27 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>